<commit_message>
updated excel sheet and screenshots of questions
</commit_message>
<xml_diff>
--- a/Car Inventory.xlsx
+++ b/Car Inventory.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/edgar/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B728A16-BC9B-8546-B253-720C857ABF49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DECE190F-C011-7543-9094-462688997AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{8DDC7C5A-E9EA-4E0E-924E-C90D51B528B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
-    <sheet name="Car Inventory" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
+    <sheet name="Car Inventory" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId4"/>
+    <pivotCache cacheId="9" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="55">
   <si>
     <t>Row Labels</t>
   </si>
@@ -159,9 +160,6 @@
     <t>2. What is the color with the largest profit margin?</t>
   </si>
   <si>
-    <t>Average of Mileage</t>
-  </si>
-  <si>
     <t>Calculated Field</t>
   </si>
   <si>
@@ -201,10 +199,13 @@
     <t>on the Options tab, in the Calculations group, click Fields, Items, &amp; Sets, and then click Solve Order.</t>
   </si>
   <si>
-    <t>1. For which model does milage matter the least?</t>
-  </si>
-  <si>
-    <t>Sum of Average Mileage Profit</t>
+    <t>1. What is the highest profit car?</t>
+  </si>
+  <si>
+    <t>Average Mileage Profit</t>
+  </si>
+  <si>
+    <t>=Mileage/'Profit Margin'</t>
   </si>
 </sst>
 </file>
@@ -281,7 +282,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
@@ -294,13 +295,49 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="12">
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     </dxf>
@@ -335,6 +372,36 @@
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:pivotFmts>
       <c:pivotFmt>
@@ -1739,6 +1806,118 @@
       </c:pivotFmt>
       <c:pivotFmt>
         <c:idx val="25"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="26"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="27"/>
         <c:spPr>
           <a:solidFill>
             <a:schemeClr val="accent1"/>
@@ -1809,7 +1988,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Average of Mileage</c:v>
+                  <c:v>Total</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1825,108 +2004,130 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$4:$A$19</c:f>
-              <c:strCache>
+            <c:multiLvlStrRef>
+              <c:f>Sheet1!$A$4:$A$25</c:f>
+              <c:multiLvlStrCache>
                 <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>Accord</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Altima</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Camry</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Charger</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Civic</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Corolla</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>CRV</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Escape</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>F-150</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Fusion</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Impala</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Malibu</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Maxima</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Mustang</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Silverado</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Impala</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Malibu</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Silverado</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Charger</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Escape</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>F-150</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Fusion</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Mustang</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Accord</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Civic</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>CRV</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Altima</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Maxima</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Camry</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Corolla</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Chevrolet</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Dodge</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Ford</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Honda</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Nissan</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Toyota</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$4:$B$19</c:f>
+              <c:f>Sheet1!$B$4:$B$25</c:f>
               <c:numCache>
                 <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>86667</c:v>
+                  <c:v>631</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>62540</c:v>
+                  <c:v>361</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>75006</c:v>
+                  <c:v>459</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>76600.333333333328</c:v>
+                  <c:v>1391</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>138789</c:v>
+                  <c:v>643</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>92377</c:v>
+                  <c:v>950</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>49326</c:v>
+                  <c:v>559</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>52042.5</c:v>
+                  <c:v>606</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>89073</c:v>
+                  <c:v>2000</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>42542</c:v>
+                  <c:v>823</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>114243</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>139300</c:v>
+                  <c:v>1296</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>101856</c:v>
+                  <c:v>414</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>41560</c:v>
+                  <c:v>298</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>109231</c:v>
+                  <c:v>882</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1934,280 +2135,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000008-2C7D-9346-A935-6928CCCF3BF3}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$C$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Sum of Profit Margin</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$4:$A$19</c:f>
-              <c:strCache>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>Accord</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Altima</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Camry</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Charger</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Civic</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Corolla</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>CRV</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Escape</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>F-150</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Fusion</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Impala</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Malibu</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Maxima</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Mustang</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Silverado</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$4:$C$19</c:f>
-              <c:numCache>
-                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1296</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>298</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1391</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>823</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>882</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>645</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>643</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>950</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>559</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>631</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>361</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>414</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>606</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>459</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000018-2C7D-9346-A935-6928CCCF3BF3}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$D$3</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Sum of Average Mileage Profit</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent3"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$A$4:$A$19</c:f>
-              <c:strCache>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>Accord</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Altima</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Camry</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Charger</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Civic</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Corolla</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>CRV</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Escape</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>F-150</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Fusion</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Impala</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Malibu</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Maxima</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>Mustang</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>Silverado</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$D$4:$D$19</c:f>
-              <c:numCache>
-                <c:formatCode>_(* #,##0_);_(* \(#,##0\);_(* "-"??_);_(@_)</c:formatCode>
-                <c:ptCount val="15"/>
-                <c:pt idx="0">
-                  <c:v>130.00049999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>96.512345679012341</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>251.69798657718121</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>165.20560747663552</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>168.63791008505467</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>314.20748299319729</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>76.474418604651163</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>161.87402799377915</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>93.761052631578949</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>76.103756708407872</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>362.10142630744849</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>385.87257617728534</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>246.02898550724638</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>68.580858085808586</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>237.97603485838781</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000019-2C7D-9346-A935-6928CCCF3BF3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3327,10 +3254,10 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F36CD9A0-7F4C-40F7-AB97-F719B0073F0D}" name="PivotTable2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A3:D19" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F36CD9A0-7F4C-40F7-AB97-F719B0073F0D}" name="PivotTable2" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A3:B25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
-    <pivotField showAll="0">
+    <pivotField axis="axisRow" showAll="0">
       <items count="7">
         <item x="4"/>
         <item x="5"/>
@@ -3372,7 +3299,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField dataField="1" numFmtId="165" showAll="0">
+    <pivotField numFmtId="165" showAll="0">
       <items count="25">
         <item x="21"/>
         <item x="16"/>
@@ -3432,109 +3359,97 @@
     </pivotField>
     <pivotField numFmtId="164" showAll="0"/>
     <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
-    <pivotField dataField="1" dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
+    <pivotField dragToRow="0" dragToCol="0" dragToPage="0" showAll="0" defaultSubtotal="0"/>
   </pivotFields>
-  <rowFields count="1">
+  <rowFields count="2">
+    <field x="0"/>
     <field x="1"/>
   </rowFields>
-  <rowItems count="16">
+  <rowItems count="22">
     <i>
       <x/>
+    </i>
+    <i r="1">
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="14"/>
     </i>
     <i>
       <x v="1"/>
     </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
     <i>
       <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="13"/>
     </i>
     <i>
       <x v="3"/>
     </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
     <i>
       <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="12"/>
     </i>
     <i>
       <x v="5"/>
     </i>
-    <i>
-      <x v="6"/>
+    <i r="1">
+      <x v="2"/>
     </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
-    </i>
-    <i>
-      <x v="12"/>
-    </i>
-    <i>
-      <x v="13"/>
-    </i>
-    <i>
-      <x v="14"/>
+    <i r="1">
+      <x v="5"/>
     </i>
     <i t="grand">
       <x/>
     </i>
   </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
+  <colItems count="1">
+    <i/>
   </colItems>
-  <dataFields count="3">
-    <dataField name="Average of Mileage" fld="3" subtotal="average" baseField="0" baseItem="0"/>
+  <dataFields count="1">
     <dataField name="Sum of Profit Margin" fld="6" baseField="0" baseItem="0" numFmtId="164"/>
-    <dataField name="Sum of Average Mileage Profit" fld="7" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="0">
+    <format dxfId="11">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
-  <chartFormats count="3">
-    <chartFormat chart="0" format="15" series="1">
+  <chartFormats count="1">
+    <chartFormat chart="0" format="24" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="24" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="1"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="25" series="1">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="1">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
           </reference>
         </references>
       </pivotArea>
@@ -3864,18 +3779,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>42</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -3883,49 +3798,49 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
         <v>44</v>
-      </c>
-      <c r="C3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
         <v>48</v>
-      </c>
-      <c r="B10" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -3934,18 +3849,113 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C623EFBF-FFDC-B24F-85FB-EA33F3758542}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8840E9D9-4C43-4F55-8F1A-810E2D2A56A4}">
   <dimension ref="A3:H27"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
@@ -3953,252 +3963,194 @@
     <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" t="s">
         <v>35</v>
       </c>
-      <c r="D3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1451</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="7">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="7">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" s="7">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="7">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="7">
+        <v>2758</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="7">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="7">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" s="7">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="7">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="7">
+        <v>3468</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="7">
-        <v>86667</v>
-      </c>
-      <c r="C4" s="7">
+      <c r="B16" s="7">
         <v>2000</v>
       </c>
-      <c r="D4" s="7">
-        <v>130.00049999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="7">
-        <v>62540</v>
-      </c>
-      <c r="C5" s="7">
-        <v>1296</v>
-      </c>
-      <c r="D5" s="7">
-        <v>96.512345679012341</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" s="7">
-        <v>75006</v>
-      </c>
-      <c r="C6" s="7">
-        <v>298</v>
-      </c>
-      <c r="D6" s="7">
-        <v>251.69798657718121</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" s="7">
-        <v>76600.333333333328</v>
-      </c>
-      <c r="C7" s="7">
-        <v>1391</v>
-      </c>
-      <c r="D7" s="7">
-        <v>165.20560747663552</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="7">
-        <v>138789</v>
-      </c>
-      <c r="C8" s="7">
+      <c r="B17" s="7">
         <v>823</v>
       </c>
-      <c r="D8" s="7">
-        <v>168.63791008505467</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="7">
-        <v>92377</v>
-      </c>
-      <c r="C9" s="7">
-        <v>882</v>
-      </c>
-      <c r="D9" s="7">
-        <v>314.20748299319729</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="7">
-        <v>49326</v>
-      </c>
-      <c r="C10" s="7">
+      <c r="B18" s="7">
         <v>645</v>
-      </c>
-      <c r="D10" s="7">
-        <v>76.474418604651163</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="7">
-        <v>52042.5</v>
-      </c>
-      <c r="C11" s="7">
-        <v>643</v>
-      </c>
-      <c r="D11" s="7">
-        <v>161.87402799377915</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="7">
-        <v>89073</v>
-      </c>
-      <c r="C12" s="7">
-        <v>950</v>
-      </c>
-      <c r="D12" s="7">
-        <v>93.761052631578949</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="7">
-        <v>42542</v>
-      </c>
-      <c r="C13" s="7">
-        <v>559</v>
-      </c>
-      <c r="D13" s="7">
-        <v>76.103756708407872</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="7">
-        <v>114243</v>
-      </c>
-      <c r="C14" s="7">
-        <v>631</v>
-      </c>
-      <c r="D14" s="7">
-        <v>362.10142630744849</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B15" s="7">
-        <v>139300</v>
-      </c>
-      <c r="C15" s="7">
-        <v>361</v>
-      </c>
-      <c r="D15" s="7">
-        <v>385.87257617728534</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B16" s="7">
-        <v>101856</v>
-      </c>
-      <c r="C16" s="7">
-        <v>414</v>
-      </c>
-      <c r="D16" s="7">
-        <v>246.02898550724638</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="7">
-        <v>41560</v>
-      </c>
-      <c r="C17" s="7">
-        <v>606</v>
-      </c>
-      <c r="D17" s="7">
-        <v>68.580858085808586</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" s="7">
-        <v>109231</v>
-      </c>
-      <c r="C18" s="7">
-        <v>459</v>
-      </c>
-      <c r="D18" s="7">
-        <v>237.97603485838781</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B19" s="7">
-        <v>83802.791666666672</v>
-      </c>
-      <c r="C19" s="7">
-        <v>11958</v>
-      </c>
-      <c r="D19" s="7">
-        <v>168.19426325472486</v>
+        <v>1710</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" s="7">
+        <v>1296</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="7">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="7">
+        <v>1180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="7">
+        <v>298</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="7">
+        <v>882</v>
+      </c>
       <c r="H24" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B25" s="7">
+        <v>11958</v>
+      </c>
       <c r="H25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
@@ -4217,11 +4169,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B3CA43-F384-4E3C-853C-EF7ADCDBB550}">
   <dimension ref="B1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>

</xml_diff>